<commit_message>
add balance tests version 6
</commit_message>
<xml_diff>
--- a/data/parishes/treated_parishes.xlsx
+++ b/data/parishes/treated_parishes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Recon\paper-3-analysis\data\parishes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanjayes/Documents/PhD/paper-3-analysis/data/parishes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78622BE-C79A-429E-B5BC-A910AD49DFAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310D12BD-5875-C149-9A06-598322F7993B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="treated_parishes" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>parish_code</t>
   </si>
   <si>
-    <t>iline</t>
-  </si>
-  <si>
     <t>parish_name_lower</t>
   </si>
   <si>
@@ -1329,6 +1326,9 @@
   </si>
   <si>
     <t>ÖDEBY FÖRSAMLING</t>
+  </si>
+  <si>
+    <t>treated</t>
   </si>
 </sst>
 </file>
@@ -2171,19 +2171,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2191,15 +2191,15 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>431</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
       </c>
       <c r="B2">
         <v>31901000</v>
@@ -2208,12 +2208,12 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
       </c>
       <c r="B3">
         <v>36001000</v>
@@ -2222,12 +2222,12 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
       </c>
       <c r="B4">
         <v>36004000</v>
@@ -2236,12 +2236,12 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
       </c>
       <c r="B5">
         <v>36005000</v>
@@ -2250,12 +2250,12 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>12</v>
       </c>
       <c r="B6">
         <v>36006000</v>
@@ -2264,12 +2264,12 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
       </c>
       <c r="B7">
         <v>36007000</v>
@@ -2278,12 +2278,12 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>16</v>
       </c>
       <c r="B8">
         <v>38214000</v>
@@ -2292,12 +2292,12 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>18</v>
       </c>
       <c r="B9">
         <v>148501000</v>
@@ -2306,12 +2306,12 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>20</v>
       </c>
       <c r="B10">
         <v>158001000</v>
@@ -2320,12 +2320,12 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>22</v>
       </c>
       <c r="B11">
         <v>158001002</v>
@@ -2334,12 +2334,12 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>24</v>
       </c>
       <c r="B12">
         <v>158002000</v>
@@ -2348,12 +2348,12 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>26</v>
       </c>
       <c r="B13">
         <v>158009000</v>
@@ -2362,12 +2362,12 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>28</v>
       </c>
       <c r="B14">
         <v>158101000</v>
@@ -2376,12 +2376,12 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>30</v>
       </c>
       <c r="B15">
         <v>158102000</v>
@@ -2390,12 +2390,12 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>32</v>
       </c>
       <c r="B16">
         <v>158103000</v>
@@ -2404,12 +2404,12 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>34</v>
       </c>
       <c r="B17">
         <v>158104000</v>
@@ -2418,12 +2418,12 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>36</v>
       </c>
       <c r="B18">
         <v>158107000</v>
@@ -2432,12 +2432,12 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>38</v>
       </c>
       <c r="B19">
         <v>160203000</v>
@@ -2446,12 +2446,12 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>40</v>
       </c>
       <c r="B20">
         <v>160204000</v>
@@ -2460,12 +2460,12 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>42</v>
       </c>
       <c r="B21">
         <v>160205000</v>
@@ -2474,12 +2474,12 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>44</v>
       </c>
       <c r="B22">
         <v>160206000</v>
@@ -2488,12 +2488,12 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>46</v>
       </c>
       <c r="B23">
         <v>160208000</v>
@@ -2502,12 +2502,12 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>48</v>
       </c>
       <c r="B24">
         <v>160209000</v>
@@ -2516,12 +2516,12 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>50</v>
       </c>
       <c r="B25">
         <v>160212000</v>
@@ -2530,12 +2530,12 @@
         <v>1</v>
       </c>
       <c r="D25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>52</v>
       </c>
       <c r="B26">
         <v>160301000</v>
@@ -2544,12 +2544,12 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>54</v>
       </c>
       <c r="B27">
         <v>160303000</v>
@@ -2558,12 +2558,12 @@
         <v>1</v>
       </c>
       <c r="D27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>56</v>
       </c>
       <c r="B28">
         <v>160304000</v>
@@ -2572,12 +2572,12 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>58</v>
       </c>
       <c r="B29">
         <v>164301000</v>
@@ -2586,12 +2586,12 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>60</v>
       </c>
       <c r="B30">
         <v>164302000</v>
@@ -2600,12 +2600,12 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>62</v>
       </c>
       <c r="B31">
         <v>164303000</v>
@@ -2614,12 +2614,12 @@
         <v>1</v>
       </c>
       <c r="D31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>64</v>
       </c>
       <c r="B32">
         <v>166001000</v>
@@ -2628,12 +2628,12 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>66</v>
       </c>
       <c r="B33">
         <v>166002000</v>
@@ -2642,12 +2642,12 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>68</v>
       </c>
       <c r="B34">
         <v>166004000</v>
@@ -2656,12 +2656,12 @@
         <v>1</v>
       </c>
       <c r="D34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>70</v>
       </c>
       <c r="B35">
         <v>166005000</v>
@@ -2670,12 +2670,12 @@
         <v>1</v>
       </c>
       <c r="D35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>72</v>
       </c>
       <c r="B36">
         <v>166006000</v>
@@ -2684,12 +2684,12 @@
         <v>1</v>
       </c>
       <c r="D36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>74</v>
       </c>
       <c r="B37">
         <v>166007000</v>
@@ -2698,12 +2698,12 @@
         <v>1</v>
       </c>
       <c r="D37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>76</v>
       </c>
       <c r="B38">
         <v>166008000</v>
@@ -2712,12 +2712,12 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>78</v>
       </c>
       <c r="B39">
         <v>166009000</v>
@@ -2726,12 +2726,12 @@
         <v>1</v>
       </c>
       <c r="D39" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>80</v>
       </c>
       <c r="B40">
         <v>166010000</v>
@@ -2740,12 +2740,12 @@
         <v>1</v>
       </c>
       <c r="D40" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>82</v>
       </c>
       <c r="B41">
         <v>166011000</v>
@@ -2754,12 +2754,12 @@
         <v>1</v>
       </c>
       <c r="D41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>84</v>
       </c>
       <c r="B42">
         <v>166014000</v>
@@ -2768,12 +2768,12 @@
         <v>1</v>
       </c>
       <c r="D42" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>86</v>
       </c>
       <c r="B43">
         <v>166015000</v>
@@ -2782,12 +2782,12 @@
         <v>1</v>
       </c>
       <c r="D43" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>88</v>
       </c>
       <c r="B44">
         <v>166024000</v>
@@ -2796,12 +2796,12 @@
         <v>1</v>
       </c>
       <c r="D44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>90</v>
       </c>
       <c r="B45">
         <v>166026000</v>
@@ -2810,12 +2810,12 @@
         <v>1</v>
       </c>
       <c r="D45" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>92</v>
       </c>
       <c r="B46">
         <v>166028000</v>
@@ -2824,12 +2824,12 @@
         <v>1</v>
       </c>
       <c r="D46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>94</v>
       </c>
       <c r="B47">
         <v>166029000</v>
@@ -2838,12 +2838,12 @@
         <v>1</v>
       </c>
       <c r="D47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>96</v>
       </c>
       <c r="B48">
         <v>166032000</v>
@@ -2852,12 +2852,12 @@
         <v>1</v>
       </c>
       <c r="D48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>98</v>
       </c>
       <c r="B49">
         <v>166101000</v>
@@ -2866,12 +2866,12 @@
         <v>1</v>
       </c>
       <c r="D49" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>100</v>
       </c>
       <c r="B50">
         <v>166102000</v>
@@ -2880,12 +2880,12 @@
         <v>1</v>
       </c>
       <c r="D50" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>102</v>
       </c>
       <c r="B51">
         <v>166106000</v>
@@ -2894,12 +2894,12 @@
         <v>1</v>
       </c>
       <c r="D51" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>104</v>
       </c>
       <c r="B52">
         <v>166112000</v>
@@ -2908,12 +2908,12 @@
         <v>1</v>
       </c>
       <c r="D52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>106</v>
       </c>
       <c r="B53">
         <v>166113000</v>
@@ -2922,12 +2922,12 @@
         <v>1</v>
       </c>
       <c r="D53" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>108</v>
       </c>
       <c r="B54">
         <v>166114000</v>
@@ -2936,12 +2936,12 @@
         <v>1</v>
       </c>
       <c r="D54" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>110</v>
       </c>
       <c r="B55">
         <v>166115000</v>
@@ -2950,12 +2950,12 @@
         <v>1</v>
       </c>
       <c r="D55" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>112</v>
       </c>
       <c r="B56">
         <v>166116000</v>
@@ -2964,12 +2964,12 @@
         <v>1</v>
       </c>
       <c r="D56" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>114</v>
       </c>
       <c r="B57">
         <v>166117000</v>
@@ -2978,12 +2978,12 @@
         <v>1</v>
       </c>
       <c r="D57" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>116</v>
       </c>
       <c r="B58">
         <v>166118000</v>
@@ -2992,12 +2992,12 @@
         <v>1</v>
       </c>
       <c r="D58" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>118</v>
       </c>
       <c r="B59">
         <v>166119000</v>
@@ -3006,12 +3006,12 @@
         <v>1</v>
       </c>
       <c r="D59" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>120</v>
       </c>
       <c r="B60">
         <v>166120000</v>
@@ -3020,12 +3020,12 @@
         <v>1</v>
       </c>
       <c r="D60" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>122</v>
       </c>
       <c r="B61">
         <v>166301000</v>
@@ -3034,12 +3034,12 @@
         <v>1</v>
       </c>
       <c r="D61" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>124</v>
       </c>
       <c r="B62">
         <v>166302000</v>
@@ -3048,12 +3048,12 @@
         <v>1</v>
       </c>
       <c r="D62" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>126</v>
       </c>
       <c r="B63">
         <v>168001000</v>
@@ -3062,12 +3062,12 @@
         <v>1</v>
       </c>
       <c r="D63" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>128</v>
       </c>
       <c r="B64">
         <v>168002000</v>
@@ -3076,12 +3076,12 @@
         <v>1</v>
       </c>
       <c r="D64" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>130</v>
       </c>
       <c r="B65">
         <v>168003000</v>
@@ -3090,12 +3090,12 @@
         <v>1</v>
       </c>
       <c r="D65" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>132</v>
       </c>
       <c r="B66">
         <v>168011000</v>
@@ -3104,12 +3104,12 @@
         <v>1</v>
       </c>
       <c r="D66" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>134</v>
       </c>
       <c r="B67">
         <v>168012000</v>
@@ -3118,12 +3118,12 @@
         <v>1</v>
       </c>
       <c r="D67" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>136</v>
       </c>
       <c r="B68">
         <v>168014000</v>
@@ -3132,12 +3132,12 @@
         <v>1</v>
       </c>
       <c r="D68" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>138</v>
       </c>
       <c r="B69">
         <v>168015000</v>
@@ -3146,12 +3146,12 @@
         <v>1</v>
       </c>
       <c r="D69" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>140</v>
       </c>
       <c r="B70">
         <v>168016000</v>
@@ -3160,12 +3160,12 @@
         <v>1</v>
       </c>
       <c r="D70" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>142</v>
       </c>
       <c r="B71">
         <v>168018000</v>
@@ -3174,12 +3174,12 @@
         <v>1</v>
       </c>
       <c r="D71" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>144</v>
       </c>
       <c r="B72">
         <v>168101000</v>
@@ -3188,12 +3188,12 @@
         <v>1</v>
       </c>
       <c r="D72" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>146</v>
       </c>
       <c r="B73">
         <v>168102000</v>
@@ -3202,12 +3202,12 @@
         <v>1</v>
       </c>
       <c r="D73" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>148</v>
       </c>
       <c r="B74">
         <v>168103000</v>
@@ -3216,12 +3216,12 @@
         <v>1</v>
       </c>
       <c r="D74" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>149</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>150</v>
       </c>
       <c r="B75">
         <v>168105000</v>
@@ -3230,12 +3230,12 @@
         <v>1</v>
       </c>
       <c r="D75" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>151</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>152</v>
       </c>
       <c r="B76">
         <v>168106000</v>
@@ -3244,12 +3244,12 @@
         <v>1</v>
       </c>
       <c r="D76" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>154</v>
       </c>
       <c r="B77">
         <v>168107000</v>
@@ -3258,12 +3258,12 @@
         <v>1</v>
       </c>
       <c r="D77" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>156</v>
       </c>
       <c r="B78">
         <v>168114000</v>
@@ -3272,12 +3272,12 @@
         <v>1</v>
       </c>
       <c r="D78" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>158</v>
       </c>
       <c r="B79">
         <v>168115000</v>
@@ -3286,12 +3286,12 @@
         <v>1</v>
       </c>
       <c r="D79" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>159</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>160</v>
       </c>
       <c r="B80">
         <v>168116000</v>
@@ -3300,12 +3300,12 @@
         <v>1</v>
       </c>
       <c r="D80" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>162</v>
       </c>
       <c r="B81">
         <v>168117000</v>
@@ -3314,12 +3314,12 @@
         <v>1</v>
       </c>
       <c r="D81" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>163</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>164</v>
       </c>
       <c r="B82">
         <v>168118000</v>
@@ -3328,12 +3328,12 @@
         <v>1</v>
       </c>
       <c r="D82" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>165</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>166</v>
       </c>
       <c r="B83">
         <v>168119000</v>
@@ -3342,12 +3342,12 @@
         <v>1</v>
       </c>
       <c r="D83" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>167</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>168</v>
       </c>
       <c r="B84">
         <v>168120000</v>
@@ -3356,12 +3356,12 @@
         <v>1</v>
       </c>
       <c r="D84" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>169</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>170</v>
       </c>
       <c r="B85">
         <v>168121000</v>
@@ -3370,12 +3370,12 @@
         <v>1</v>
       </c>
       <c r="D85" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>172</v>
       </c>
       <c r="B86">
         <v>168122000</v>
@@ -3384,12 +3384,12 @@
         <v>1</v>
       </c>
       <c r="D86" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>174</v>
       </c>
       <c r="B87">
         <v>168124000</v>
@@ -3398,12 +3398,12 @@
         <v>1</v>
       </c>
       <c r="D87" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>176</v>
       </c>
       <c r="B88">
         <v>168126000</v>
@@ -3412,12 +3412,12 @@
         <v>1</v>
       </c>
       <c r="D88" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>178</v>
       </c>
       <c r="B89">
         <v>168127000</v>
@@ -3426,12 +3426,12 @@
         <v>1</v>
       </c>
       <c r="D89" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>180</v>
       </c>
       <c r="B90">
         <v>168201001</v>
@@ -3440,12 +3440,12 @@
         <v>1</v>
       </c>
       <c r="D90" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>181</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>182</v>
       </c>
       <c r="B91">
         <v>168201002</v>
@@ -3454,12 +3454,12 @@
         <v>1</v>
       </c>
       <c r="D91" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
         <v>183</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>184</v>
       </c>
       <c r="B92">
         <v>168202000</v>
@@ -3468,12 +3468,12 @@
         <v>1</v>
       </c>
       <c r="D92" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>185</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>186</v>
       </c>
       <c r="B93">
         <v>168204000</v>
@@ -3482,12 +3482,12 @@
         <v>1</v>
       </c>
       <c r="D93" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>187</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>188</v>
       </c>
       <c r="B94">
         <v>168205000</v>
@@ -3496,12 +3496,12 @@
         <v>1</v>
       </c>
       <c r="D94" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>189</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>190</v>
       </c>
       <c r="B95">
         <v>168207000</v>
@@ -3510,12 +3510,12 @@
         <v>1</v>
       </c>
       <c r="D95" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
         <v>191</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>192</v>
       </c>
       <c r="B96">
         <v>168208000</v>
@@ -3524,12 +3524,12 @@
         <v>1</v>
       </c>
       <c r="D96" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
         <v>193</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>194</v>
       </c>
       <c r="B97">
         <v>168209000</v>
@@ -3538,12 +3538,12 @@
         <v>1</v>
       </c>
       <c r="D97" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
         <v>195</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>196</v>
       </c>
       <c r="B98">
         <v>168210000</v>
@@ -3552,12 +3552,12 @@
         <v>1</v>
       </c>
       <c r="D98" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
         <v>197</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>198</v>
       </c>
       <c r="B99">
         <v>168211000</v>
@@ -3566,12 +3566,12 @@
         <v>1</v>
       </c>
       <c r="D99" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
         <v>199</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>200</v>
       </c>
       <c r="B100">
         <v>168212000</v>
@@ -3580,12 +3580,12 @@
         <v>1</v>
       </c>
       <c r="D100" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
         <v>201</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>202</v>
       </c>
       <c r="B101">
         <v>168214000</v>
@@ -3594,12 +3594,12 @@
         <v>1</v>
       </c>
       <c r="D101" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
         <v>203</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>204</v>
       </c>
       <c r="B102">
         <v>168214002</v>
@@ -3608,12 +3608,12 @@
         <v>1</v>
       </c>
       <c r="D102" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
         <v>205</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>206</v>
       </c>
       <c r="B103">
         <v>168217000</v>
@@ -3622,12 +3622,12 @@
         <v>1</v>
       </c>
       <c r="D103" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
         <v>207</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>208</v>
       </c>
       <c r="B104">
         <v>168301003</v>
@@ -3636,12 +3636,12 @@
         <v>1</v>
       </c>
       <c r="D104" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
         <v>209</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>210</v>
       </c>
       <c r="B105">
         <v>168303000</v>
@@ -3650,12 +3650,12 @@
         <v>1</v>
       </c>
       <c r="D105" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
         <v>211</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>212</v>
       </c>
       <c r="B106">
         <v>168304000</v>
@@ -3664,12 +3664,12 @@
         <v>1</v>
       </c>
       <c r="D106" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
         <v>213</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>214</v>
       </c>
       <c r="B107">
         <v>168305000</v>
@@ -3678,12 +3678,12 @@
         <v>1</v>
       </c>
       <c r="D107" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
         <v>215</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>216</v>
       </c>
       <c r="B108">
         <v>168306000</v>
@@ -3692,12 +3692,12 @@
         <v>1</v>
       </c>
       <c r="D108" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
         <v>217</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>218</v>
       </c>
       <c r="B109">
         <v>168308000</v>
@@ -3706,12 +3706,12 @@
         <v>1</v>
       </c>
       <c r="D109" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
         <v>219</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>220</v>
       </c>
       <c r="B110">
         <v>168601001</v>
@@ -3720,12 +3720,12 @@
         <v>1</v>
       </c>
       <c r="D110" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
         <v>221</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>222</v>
       </c>
       <c r="B111">
         <v>168601002</v>
@@ -3734,12 +3734,12 @@
         <v>1</v>
       </c>
       <c r="D111" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
         <v>223</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>224</v>
       </c>
       <c r="B112">
         <v>168602000</v>
@@ -3748,12 +3748,12 @@
         <v>1</v>
       </c>
       <c r="D112" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
         <v>225</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>226</v>
       </c>
       <c r="B113">
         <v>168610000</v>
@@ -3762,12 +3762,12 @@
         <v>1</v>
       </c>
       <c r="D113" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
         <v>227</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>228</v>
       </c>
       <c r="B114">
         <v>168634000</v>
@@ -3776,12 +3776,12 @@
         <v>1</v>
       </c>
       <c r="D114" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
         <v>229</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>230</v>
       </c>
       <c r="B115">
         <v>168635000</v>
@@ -3790,12 +3790,12 @@
         <v>1</v>
       </c>
       <c r="D115" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
         <v>231</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>232</v>
       </c>
       <c r="B116">
         <v>168642000</v>
@@ -3804,12 +3804,12 @@
         <v>1</v>
       </c>
       <c r="D116" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
         <v>233</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>234</v>
       </c>
       <c r="B117">
         <v>168643000</v>
@@ -3818,12 +3818,12 @@
         <v>1</v>
       </c>
       <c r="D117" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
         <v>235</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>236</v>
       </c>
       <c r="B118">
         <v>168644000</v>
@@ -3832,12 +3832,12 @@
         <v>1</v>
       </c>
       <c r="D118" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
         <v>237</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>238</v>
       </c>
       <c r="B119">
         <v>178101000</v>
@@ -3846,12 +3846,12 @@
         <v>1</v>
       </c>
       <c r="D119" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
         <v>239</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>240</v>
       </c>
       <c r="B120">
         <v>178101002</v>
@@ -3860,12 +3860,12 @@
         <v>1</v>
       </c>
       <c r="D120" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
         <v>241</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>242</v>
       </c>
       <c r="B121">
         <v>178103000</v>
@@ -3874,12 +3874,12 @@
         <v>1</v>
       </c>
       <c r="D121" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
         <v>243</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>244</v>
       </c>
       <c r="B122">
         <v>178105000</v>
@@ -3888,12 +3888,12 @@
         <v>1</v>
       </c>
       <c r="D122" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
         <v>245</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>246</v>
       </c>
       <c r="B123">
         <v>186101000</v>
@@ -3902,12 +3902,12 @@
         <v>1</v>
       </c>
       <c r="D123" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
         <v>247</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>248</v>
       </c>
       <c r="B124">
         <v>186104000</v>
@@ -3916,12 +3916,12 @@
         <v>1</v>
       </c>
       <c r="D124" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
         <v>249</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>250</v>
       </c>
       <c r="B125">
         <v>186105000</v>
@@ -3930,12 +3930,12 @@
         <v>1</v>
       </c>
       <c r="D125" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
         <v>251</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>252</v>
       </c>
       <c r="B126">
         <v>186202000</v>
@@ -3944,12 +3944,12 @@
         <v>1</v>
       </c>
       <c r="D126" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
         <v>253</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>254</v>
       </c>
       <c r="B127">
         <v>188001001</v>
@@ -3958,12 +3958,12 @@
         <v>1</v>
       </c>
       <c r="D127" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
         <v>255</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>256</v>
       </c>
       <c r="B128">
         <v>188003000</v>
@@ -3972,12 +3972,12 @@
         <v>1</v>
       </c>
       <c r="D128" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
         <v>257</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>258</v>
       </c>
       <c r="B129">
         <v>188003005</v>
@@ -3986,12 +3986,12 @@
         <v>1</v>
       </c>
       <c r="D129" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
         <v>259</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>260</v>
       </c>
       <c r="B130">
         <v>188004000</v>
@@ -4000,12 +4000,12 @@
         <v>1</v>
       </c>
       <c r="D130" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
         <v>261</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>262</v>
       </c>
       <c r="B131">
         <v>188006000</v>
@@ -4014,12 +4014,12 @@
         <v>1</v>
       </c>
       <c r="D131" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
         <v>263</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>264</v>
       </c>
       <c r="B132">
         <v>188007000</v>
@@ -4028,12 +4028,12 @@
         <v>1</v>
       </c>
       <c r="D132" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
         <v>265</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>266</v>
       </c>
       <c r="B133">
         <v>188008000</v>
@@ -4042,12 +4042,12 @@
         <v>1</v>
       </c>
       <c r="D133" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
         <v>267</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>268</v>
       </c>
       <c r="B134">
         <v>188009000</v>
@@ -4056,12 +4056,12 @@
         <v>1</v>
       </c>
       <c r="D134" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
         <v>269</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>270</v>
       </c>
       <c r="B135">
         <v>188019000</v>
@@ -4070,12 +4070,12 @@
         <v>1</v>
       </c>
       <c r="D135" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
         <v>271</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>272</v>
       </c>
       <c r="B136">
         <v>188020000</v>
@@ -4084,12 +4084,12 @@
         <v>1</v>
       </c>
       <c r="D136" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
         <v>273</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>274</v>
       </c>
       <c r="B137">
         <v>188021000</v>
@@ -4098,12 +4098,12 @@
         <v>1</v>
       </c>
       <c r="D137" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
         <v>275</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>276</v>
       </c>
       <c r="B138">
         <v>188022000</v>
@@ -4112,12 +4112,12 @@
         <v>1</v>
       </c>
       <c r="D138" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
         <v>277</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>278</v>
       </c>
       <c r="B139">
         <v>188023000</v>
@@ -4126,12 +4126,12 @@
         <v>1</v>
       </c>
       <c r="D139" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
         <v>279</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>280</v>
       </c>
       <c r="B140">
         <v>188025000</v>
@@ -4140,12 +4140,12 @@
         <v>1</v>
       </c>
       <c r="D140" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
         <v>281</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>282</v>
       </c>
       <c r="B141">
         <v>188101000</v>
@@ -4154,12 +4154,12 @@
         <v>1</v>
       </c>
       <c r="D141" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
         <v>283</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>284</v>
       </c>
       <c r="B142">
         <v>188102000</v>
@@ -4168,12 +4168,12 @@
         <v>1</v>
       </c>
       <c r="D142" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
         <v>285</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>286</v>
       </c>
       <c r="B143">
         <v>188103000</v>
@@ -4182,12 +4182,12 @@
         <v>1</v>
       </c>
       <c r="D143" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
         <v>287</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>288</v>
       </c>
       <c r="B144">
         <v>188301000</v>
@@ -4196,12 +4196,12 @@
         <v>1</v>
       </c>
       <c r="D144" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
         <v>289</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>290</v>
       </c>
       <c r="B145">
         <v>190401000</v>
@@ -4210,12 +4210,12 @@
         <v>1</v>
       </c>
       <c r="D145" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
         <v>291</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>292</v>
       </c>
       <c r="B146">
         <v>190402000</v>
@@ -4224,12 +4224,12 @@
         <v>1</v>
       </c>
       <c r="D146" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
         <v>293</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>294</v>
       </c>
       <c r="B147">
         <v>190403000</v>
@@ -4238,12 +4238,12 @@
         <v>1</v>
       </c>
       <c r="D147" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
         <v>295</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>296</v>
       </c>
       <c r="B148">
         <v>190701000</v>
@@ -4252,12 +4252,12 @@
         <v>1</v>
       </c>
       <c r="D148" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
         <v>297</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>298</v>
       </c>
       <c r="B149">
         <v>190702000</v>
@@ -4266,12 +4266,12 @@
         <v>1</v>
       </c>
       <c r="D149" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
         <v>299</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>300</v>
       </c>
       <c r="B150">
         <v>196101000</v>
@@ -4280,12 +4280,12 @@
         <v>1</v>
       </c>
       <c r="D150" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
         <v>301</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>302</v>
       </c>
       <c r="B151">
         <v>196102000</v>
@@ -4294,12 +4294,12 @@
         <v>1</v>
       </c>
       <c r="D151" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
         <v>303</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>304</v>
       </c>
       <c r="B152">
         <v>196103000</v>
@@ -4308,12 +4308,12 @@
         <v>1</v>
       </c>
       <c r="D152" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
         <v>305</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>306</v>
       </c>
       <c r="B153">
         <v>196201000</v>
@@ -4322,12 +4322,12 @@
         <v>1</v>
       </c>
       <c r="D153" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
         <v>307</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>308</v>
       </c>
       <c r="B154">
         <v>198001000</v>
@@ -4336,12 +4336,12 @@
         <v>1</v>
       </c>
       <c r="D154" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
         <v>309</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>310</v>
       </c>
       <c r="B155">
         <v>198002000</v>
@@ -4350,12 +4350,12 @@
         <v>1</v>
       </c>
       <c r="D155" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
         <v>311</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>312</v>
       </c>
       <c r="B156">
         <v>198003000</v>
@@ -4364,12 +4364,12 @@
         <v>1</v>
       </c>
       <c r="D156" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
         <v>313</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>314</v>
       </c>
       <c r="B157">
         <v>198004001</v>
@@ -4378,12 +4378,12 @@
         <v>1</v>
       </c>
       <c r="D157" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
         <v>315</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>316</v>
       </c>
       <c r="B158">
         <v>198004002</v>
@@ -4392,12 +4392,12 @@
         <v>1</v>
       </c>
       <c r="D158" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
         <v>317</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>318</v>
       </c>
       <c r="B159">
         <v>198006000</v>
@@ -4406,12 +4406,12 @@
         <v>1</v>
       </c>
       <c r="D159" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
         <v>319</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>320</v>
       </c>
       <c r="B160">
         <v>198007000</v>
@@ -4420,12 +4420,12 @@
         <v>1</v>
       </c>
       <c r="D160" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
         <v>321</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>322</v>
       </c>
       <c r="B161">
         <v>198008000</v>
@@ -4434,12 +4434,12 @@
         <v>1</v>
       </c>
       <c r="D161" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
         <v>323</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>324</v>
       </c>
       <c r="B162">
         <v>198009000</v>
@@ -4448,12 +4448,12 @@
         <v>1</v>
       </c>
       <c r="D162" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
         <v>325</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>326</v>
       </c>
       <c r="B163">
         <v>198016000</v>
@@ -4462,12 +4462,12 @@
         <v>1</v>
       </c>
       <c r="D163" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
         <v>327</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>328</v>
       </c>
       <c r="B164">
         <v>198017000</v>
@@ -4476,12 +4476,12 @@
         <v>1</v>
       </c>
       <c r="D164" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
         <v>329</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>330</v>
       </c>
       <c r="B165">
         <v>198101002</v>
@@ -4490,12 +4490,12 @@
         <v>1</v>
       </c>
       <c r="D165" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
         <v>331</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>332</v>
       </c>
       <c r="B166">
         <v>198106000</v>
@@ -4504,12 +4504,12 @@
         <v>1</v>
       </c>
       <c r="D166" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B167">
         <v>198107000</v>
@@ -4518,12 +4518,12 @@
         <v>1</v>
       </c>
       <c r="D167" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
         <v>334</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>335</v>
       </c>
       <c r="B168">
         <v>198201000</v>
@@ -4532,12 +4532,12 @@
         <v>1</v>
       </c>
       <c r="D168" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
         <v>336</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>337</v>
       </c>
       <c r="B169">
         <v>198202000</v>
@@ -4546,12 +4546,12 @@
         <v>1</v>
       </c>
       <c r="D169" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
         <v>338</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>339</v>
       </c>
       <c r="B170">
         <v>198304001</v>
@@ -4560,12 +4560,12 @@
         <v>1</v>
       </c>
       <c r="D170" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
         <v>340</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>341</v>
       </c>
       <c r="B171">
         <v>198304002</v>
@@ -4574,12 +4574,12 @@
         <v>1</v>
       </c>
       <c r="D171" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B172">
         <v>198305000</v>
@@ -4588,12 +4588,12 @@
         <v>1</v>
       </c>
       <c r="D172" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
         <v>343</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>344</v>
       </c>
       <c r="B173">
         <v>208301002</v>
@@ -4602,12 +4602,12 @@
         <v>1</v>
       </c>
       <c r="D173" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
         <v>345</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>346</v>
       </c>
       <c r="B174">
         <v>208301003</v>
@@ -4616,12 +4616,12 @@
         <v>1</v>
       </c>
       <c r="D174" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
         <v>347</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>348</v>
       </c>
       <c r="B175">
         <v>208302000</v>
@@ -4630,12 +4630,12 @@
         <v>1</v>
       </c>
       <c r="D175" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
         <v>349</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>350</v>
       </c>
       <c r="B176">
         <v>208371000</v>
@@ -4644,12 +4644,12 @@
         <v>1</v>
       </c>
       <c r="D176" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
         <v>351</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>352</v>
       </c>
       <c r="B177">
         <v>208401000</v>
@@ -4658,12 +4658,12 @@
         <v>1</v>
       </c>
       <c r="D177" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
         <v>353</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>354</v>
       </c>
       <c r="B178">
         <v>208406000</v>
@@ -4672,12 +4672,12 @@
         <v>1</v>
       </c>
       <c r="D178" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
         <v>355</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>356</v>
       </c>
       <c r="B179">
         <v>208471000</v>
@@ -4686,12 +4686,12 @@
         <v>1</v>
       </c>
       <c r="D179" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
         <v>357</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>358</v>
       </c>
       <c r="B180">
         <v>208472000</v>
@@ -4700,12 +4700,12 @@
         <v>1</v>
       </c>
       <c r="D180" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
         <v>359</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>360</v>
       </c>
       <c r="B181">
         <v>210402000</v>
@@ -4714,12 +4714,12 @@
         <v>1</v>
       </c>
       <c r="D181" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
         <v>361</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>362</v>
       </c>
       <c r="B182">
         <v>218001001</v>
@@ -4728,12 +4728,12 @@
         <v>1</v>
       </c>
       <c r="D182" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
         <v>363</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>364</v>
       </c>
       <c r="B183">
         <v>218006000</v>
@@ -4742,12 +4742,12 @@
         <v>1</v>
       </c>
       <c r="D183" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
         <v>365</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>366</v>
       </c>
       <c r="B184">
         <v>218101000</v>
@@ -4756,12 +4756,12 @@
         <v>1</v>
       </c>
       <c r="D184" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
         <v>367</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>368</v>
       </c>
       <c r="B185">
         <v>218102000</v>
@@ -4770,12 +4770,12 @@
         <v>1</v>
       </c>
       <c r="D185" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
         <v>369</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>370</v>
       </c>
       <c r="B186">
         <v>218104000</v>
@@ -4784,12 +4784,12 @@
         <v>1</v>
       </c>
       <c r="D186" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
         <v>371</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>372</v>
       </c>
       <c r="B187">
         <v>218105000</v>
@@ -4798,12 +4798,12 @@
         <v>1</v>
       </c>
       <c r="D187" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B188">
         <v>188404000</v>
@@ -4812,12 +4812,12 @@
         <v>1</v>
       </c>
       <c r="D188" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B189">
         <v>188502005</v>
@@ -4826,12 +4826,12 @@
         <v>1</v>
       </c>
       <c r="D189" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B190">
         <v>188507000</v>
@@ -4840,12 +4840,12 @@
         <v>1</v>
       </c>
       <c r="D190" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B191">
         <v>188010000</v>
@@ -4854,12 +4854,12 @@
         <v>1</v>
       </c>
       <c r="D191" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B192">
         <v>188001001</v>
@@ -4868,12 +4868,12 @@
         <v>1</v>
       </c>
       <c r="D192" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B193">
         <v>188005000</v>
@@ -4882,12 +4882,12 @@
         <v>1</v>
       </c>
       <c r="D193" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B194">
         <v>188026000</v>
@@ -4896,12 +4896,12 @@
         <v>1</v>
       </c>
       <c r="D194" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B195">
         <v>188027000</v>
@@ -4910,12 +4910,12 @@
         <v>1</v>
       </c>
       <c r="D195" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B196">
         <v>188029001</v>
@@ -4924,12 +4924,12 @@
         <v>1</v>
       </c>
       <c r="D196" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B197">
         <v>188003004</v>
@@ -4938,12 +4938,12 @@
         <v>1</v>
       </c>
       <c r="D197" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B198">
         <v>188013000</v>
@@ -4952,12 +4952,12 @@
         <v>1</v>
       </c>
       <c r="D198" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B199">
         <v>188012000</v>
@@ -4966,12 +4966,12 @@
         <v>1</v>
       </c>
       <c r="D199" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B200">
         <v>188011000</v>
@@ -4980,12 +4980,12 @@
         <v>1</v>
       </c>
       <c r="D200" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B201">
         <v>198302000</v>
@@ -4994,12 +4994,12 @@
         <v>1</v>
       </c>
       <c r="D201" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B202">
         <v>198403000</v>
@@ -5008,12 +5008,12 @@
         <v>1</v>
       </c>
       <c r="D202" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B203">
         <v>188505000</v>
@@ -5022,12 +5022,12 @@
         <v>1</v>
       </c>
       <c r="D203" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B204">
         <v>198303000</v>
@@ -5036,12 +5036,12 @@
         <v>1</v>
       </c>
       <c r="D204" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B205">
         <v>188507000</v>
@@ -5050,12 +5050,12 @@
         <v>1</v>
       </c>
       <c r="D205" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B206">
         <v>198306000</v>
@@ -5064,12 +5064,12 @@
         <v>1</v>
       </c>
       <c r="D206" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B207">
         <v>198020000</v>
@@ -5078,12 +5078,12 @@
         <v>1</v>
       </c>
       <c r="D207" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B208">
         <v>198010000</v>
@@ -5092,12 +5092,12 @@
         <v>1</v>
       </c>
       <c r="D208" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B209">
         <v>218004000</v>
@@ -5106,12 +5106,12 @@
         <v>1</v>
       </c>
       <c r="D209" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B210">
         <v>198005000</v>
@@ -5120,12 +5120,12 @@
         <v>1</v>
       </c>
       <c r="D210" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B211">
         <v>198103000</v>
@@ -5134,12 +5134,12 @@
         <v>1</v>
       </c>
       <c r="D211" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B212">
         <v>198102000</v>
@@ -5148,12 +5148,12 @@
         <v>1</v>
       </c>
       <c r="D212" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B213">
         <v>196202000</v>
@@ -5162,12 +5162,12 @@
         <v>1</v>
       </c>
       <c r="D213" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B214">
         <v>198108000</v>
@@ -5176,12 +5176,12 @@
         <v>1</v>
       </c>
       <c r="D214" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B215">
         <v>196004000</v>
@@ -5190,12 +5190,12 @@
         <v>1</v>
       </c>
       <c r="D215" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B216">
         <v>188504000</v>
@@ -5204,12 +5204,12 @@
         <v>1</v>
       </c>
       <c r="D216" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B217">
         <v>188011000</v>
@@ -5218,12 +5218,12 @@
         <v>1</v>
       </c>
       <c r="D217" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B218">
         <v>188505000</v>
@@ -5232,12 +5232,12 @@
         <v>1</v>
       </c>
       <c r="D218" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B219">
         <v>188029002</v>
@@ -5246,7 +5246,7 @@
         <v>1</v>
       </c>
       <c r="D219" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
   </sheetData>

</xml_diff>